<commit_message>
multiplyng factors by bos kor
</commit_message>
<xml_diff>
--- a/default_settings/Config.xlsx
+++ b/default_settings/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JADE\Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JADE-linux\Code\default_settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27AF79B7-D000-49C8-9E25-1C46A58E1834}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F53DF02-DFB7-4DE6-8CF1-716304A558CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{B0A3356C-3012-4321-B248-DE86B5D58E08}"/>
   </bookViews>
   <sheets>
     <sheet name="MAIN Config." sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="80">
   <si>
     <t>xsdir Path</t>
   </si>
@@ -262,6 +262,12 @@
   </si>
   <si>
     <t>42c</t>
+  </si>
+  <si>
+    <t>ASPIS Iron-88 benchmark</t>
+  </si>
+  <si>
+    <t>ASPIS-Fe88</t>
   </si>
 </sst>
 </file>
@@ -419,7 +425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -493,6 +499,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -887,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51291A71-4ED6-4F39-B575-920D7DB78E56}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1166,10 +1175,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8EEB530-2BB1-44BD-96B5-AB98331CD0CC}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1411,10 +1420,10 @@
         <v>30</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F10" s="12">
         <v>1000000000</v>
@@ -1431,7 +1440,7 @@
         <v>76</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>29</v>
@@ -1443,6 +1452,32 @@
         <v>50000000</v>
       </c>
       <c r="J11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="12">
+        <v>100000000</v>
+      </c>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="28" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>